<commit_message>
dashboard e anailise de qee
</commit_message>
<xml_diff>
--- a/USC - CANOAS.xlsx
+++ b/USC - CANOAS.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilvan Barbosa\PycharmProjects\Dashboard - Usina Santa Clotilde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F03537A-F233-4D0C-9FD6-7993518CD266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCAF67-0E1B-4691-8FAF-768CD9EC275D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" activeTab="1" xr2:uid="{B02BADF4-0850-4713-B9F1-5620B94019FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B02BADF4-0850-4713-B9F1-5620B94019FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Unidades" sheetId="1" r:id="rId1"/>
     <sheet name="Valor" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unidades!$A$1:$O$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unidades!$A$1:$P$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Mês</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Consumo Reativo Reservado (kVAr)</t>
   </si>
   <si>
-    <t>Meta Consumo Ativo Reservado (kWh)</t>
-  </si>
-  <si>
     <t>Diferença Demanda (kW)</t>
   </si>
   <si>
@@ -125,12 +122,21 @@
   </si>
   <si>
     <t>Demanda de Ultrapassagem (kW)</t>
+  </si>
+  <si>
+    <t>Meta Consumo Ativo Reservado (%)</t>
+  </si>
+  <si>
+    <t>Consumo Reservado (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -378,19 +384,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -404,11 +397,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -431,12 +425,6 @@
     <xf numFmtId="17" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,7 +437,7 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,13 +454,30 @@
     <xf numFmtId="2" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -806,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ACD048-E26D-43F8-8A45-756E0CC9B87A}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,17 +823,17 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,547 +850,610 @@
         <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>45444</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>10464.299999999999</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>864.15</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <v>3827.25</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="8">
         <f>B2+C2+D2</f>
         <v>15155.699999999999</v>
       </c>
-      <c r="F2" s="10">
-        <f>E2*(9/20)</f>
-        <v>6820.0649999999996</v>
-      </c>
-      <c r="G2" s="10">
+      <c r="F2" s="23">
+        <f>IFERROR(D2/E2*100,"")</f>
+        <v>25.252875155881949</v>
+      </c>
+      <c r="G2" s="23">
+        <f>(9/20)*100</f>
+        <v>45</v>
+      </c>
+      <c r="H2" s="8">
         <v>11750.55</v>
       </c>
-      <c r="H2" s="10">
+      <c r="I2" s="8">
         <v>1685.25</v>
       </c>
-      <c r="I2" s="10">
+      <c r="J2" s="8">
         <v>3068.1</v>
       </c>
-      <c r="J2" s="10">
-        <f>SUM(G2:I2)</f>
+      <c r="K2" s="8">
+        <f>SUM(H2:J2)</f>
         <v>16503.899999999998</v>
       </c>
-      <c r="K2" s="10">
+      <c r="L2" s="8">
         <v>315</v>
       </c>
-      <c r="L2" s="10">
+      <c r="M2" s="8">
         <v>50.4</v>
       </c>
-      <c r="M2" s="10">
+      <c r="N2" s="8">
         <v>0</v>
       </c>
-      <c r="N2" s="10">
+      <c r="O2" s="8">
         <v>300</v>
       </c>
-      <c r="O2" s="11">
-        <f t="shared" ref="O2:O13" si="0">IF(K2="","",N2-K2)</f>
+      <c r="P2" s="9">
+        <f t="shared" ref="P2:P13" si="0">IF(L2="","",O2-L2)</f>
         <v>-15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>45474</v>
-      </c>
-      <c r="B3" s="10">
+        <f t="shared" ref="A3:A13" si="1">IF(B3="","",A2+31)</f>
+        <v>45475</v>
+      </c>
+      <c r="B3" s="8">
         <v>19685.400000000001</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>1031.0999999999999</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>10178.700000000001</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" ref="E3:E8" si="1">B3+C3+D3</f>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E8" si="2">B3+C3+D3</f>
         <v>30895.200000000001</v>
       </c>
-      <c r="F3" s="10">
-        <f t="shared" ref="F3:F8" si="2">E3*(9/20)</f>
-        <v>13902.84</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="F3" s="23">
+        <f>IFERROR(D3/E3*100,"")</f>
+        <v>32.945894507884724</v>
+      </c>
+      <c r="G3" s="23">
+        <f>(9/20)*100</f>
+        <v>45</v>
+      </c>
+      <c r="H3" s="8">
         <v>12323.85</v>
       </c>
-      <c r="H3" s="10">
+      <c r="I3" s="8">
         <v>1975.05</v>
       </c>
-      <c r="I3" s="10">
+      <c r="J3" s="8">
         <v>3487.05</v>
       </c>
-      <c r="J3" s="10">
-        <f t="shared" ref="J3:J8" si="3">SUM(G3:I3)</f>
+      <c r="K3" s="8">
+        <f t="shared" ref="K3:K8" si="3">SUM(H3:J3)</f>
         <v>17785.95</v>
       </c>
-      <c r="K3" s="10">
+      <c r="L3" s="8">
         <v>319.2</v>
       </c>
-      <c r="L3" s="10">
+      <c r="M3" s="8">
         <v>1.05</v>
       </c>
-      <c r="M3" s="10">
-        <f t="shared" ref="M3:M13" si="4">IF(O3&gt;0,"",IF(SQRT(O3^2)&gt;N3*0.05,SQRT(O3^2),""))</f>
+      <c r="N3" s="8">
+        <f t="shared" ref="N3:N13" si="4">IF(P3&gt;0,"",IF(SQRT(P3^2)&gt;O3*0.05,SQRT(P3^2),""))</f>
         <v>19.199999999999989</v>
       </c>
-      <c r="N3" s="10">
+      <c r="O3" s="8">
         <v>300</v>
       </c>
-      <c r="O3" s="11">
+      <c r="P3" s="9">
         <f t="shared" si="0"/>
         <v>-19.199999999999989</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>45505</v>
-      </c>
-      <c r="B4" s="12">
+        <f t="shared" si="1"/>
+        <v>45506</v>
+      </c>
+      <c r="B4" s="10">
         <v>90227.55</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>937.65</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>59176.95</v>
       </c>
-      <c r="E4" s="12">
-        <f t="shared" si="1"/>
+      <c r="E4" s="10">
+        <f t="shared" si="2"/>
         <v>150342.15</v>
       </c>
-      <c r="F4" s="12">
-        <f t="shared" si="2"/>
-        <v>67653.967499999999</v>
-      </c>
-      <c r="G4" s="12">
+      <c r="F4" s="24">
+        <f t="shared" ref="F4:F8" si="5">IFERROR(D4/E4*100,"")</f>
+        <v>39.361516381134635</v>
+      </c>
+      <c r="G4" s="24">
+        <f t="shared" ref="G4:G8" si="6">(9/20)*100</f>
+        <v>45</v>
+      </c>
+      <c r="H4" s="10">
         <v>14696.85</v>
       </c>
-      <c r="H4" s="12">
+      <c r="I4" s="10">
         <v>984.9</v>
       </c>
-      <c r="I4" s="20">
+      <c r="J4" s="18">
         <v>3895.5</v>
       </c>
-      <c r="J4" s="12">
+      <c r="K4" s="10">
         <f t="shared" si="3"/>
         <v>19577.25</v>
       </c>
-      <c r="K4" s="21">
+      <c r="L4" s="10">
         <v>340.2</v>
       </c>
-      <c r="L4" s="12">
+      <c r="M4" s="10">
         <v>66.150000000000006</v>
       </c>
-      <c r="M4" s="12">
+      <c r="N4" s="10">
         <f t="shared" si="4"/>
         <v>40.199999999999989</v>
       </c>
-      <c r="N4" s="12">
+      <c r="O4" s="10">
         <v>300</v>
       </c>
-      <c r="O4" s="17">
+      <c r="P4" s="15">
         <f t="shared" si="0"/>
         <v>-40.199999999999989</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>45536</v>
-      </c>
-      <c r="B5" s="13">
+        <f t="shared" si="1"/>
+        <v>45537</v>
+      </c>
+      <c r="B5" s="11">
         <v>144938.85</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>1424.85</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <v>91366.8</v>
       </c>
-      <c r="E5" s="13">
-        <f t="shared" si="1"/>
+      <c r="E5" s="11">
+        <f t="shared" si="2"/>
         <v>237730.5</v>
       </c>
-      <c r="F5" s="13">
-        <f>E5*(9/20)</f>
-        <v>106978.72500000001</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="F5" s="25">
+        <f t="shared" si="5"/>
+        <v>38.432931407623336</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H5" s="11">
         <v>20242.95</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="11">
         <v>1882.65</v>
       </c>
-      <c r="I5" s="13">
+      <c r="J5" s="11">
         <v>4562.25</v>
       </c>
-      <c r="J5" s="13">
+      <c r="K5" s="11">
         <f t="shared" si="3"/>
         <v>26687.850000000002</v>
       </c>
-      <c r="K5" s="13">
+      <c r="L5" s="11">
         <v>1058.4000000000001</v>
       </c>
-      <c r="L5" s="13">
+      <c r="M5" s="11">
         <v>87.15</v>
       </c>
-      <c r="M5" s="13">
+      <c r="N5" s="11">
         <f t="shared" si="4"/>
         <v>58.400000000000091</v>
       </c>
-      <c r="N5" s="13">
+      <c r="O5" s="11">
         <v>1000</v>
       </c>
-      <c r="O5" s="16">
+      <c r="P5" s="14">
         <f t="shared" si="0"/>
         <v>-58.400000000000091</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>45566</v>
-      </c>
-      <c r="B6" s="10">
+        <f t="shared" si="1"/>
+        <v>45568</v>
+      </c>
+      <c r="B6" s="8">
         <v>114662.1</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>81.900000000000006</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>84091.35</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="1"/>
+      <c r="E6" s="8">
+        <f t="shared" si="2"/>
         <v>198835.35</v>
       </c>
-      <c r="F6" s="10">
-        <f t="shared" si="2"/>
-        <v>89475.907500000001</v>
-      </c>
-      <c r="G6" s="10">
+      <c r="F6" s="23">
+        <f t="shared" si="5"/>
+        <v>42.291951607196609</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H6" s="8">
         <v>13742.4</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="8">
         <v>79.8</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="8">
         <v>3607.8</v>
       </c>
-      <c r="J6" s="10">
+      <c r="K6" s="8">
         <f t="shared" si="3"/>
         <v>17430</v>
       </c>
-      <c r="K6" s="10">
+      <c r="L6" s="8">
         <v>1104.5999999999999</v>
       </c>
-      <c r="L6" s="10">
+      <c r="M6" s="8">
         <v>70.349999999999994</v>
       </c>
-      <c r="M6" s="10">
+      <c r="N6" s="8">
         <f t="shared" si="4"/>
         <v>104.59999999999991</v>
       </c>
-      <c r="N6" s="10">
+      <c r="O6" s="8">
         <v>1000</v>
       </c>
-      <c r="O6" s="11">
+      <c r="P6" s="9">
         <f t="shared" si="0"/>
         <v>-104.59999999999991</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>45597</v>
-      </c>
-      <c r="B7" s="10">
+        <f t="shared" si="1"/>
+        <v>45599</v>
+      </c>
+      <c r="B7" s="8">
         <v>109979.1</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>0</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>73286.850000000006</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="1"/>
+      <c r="E7" s="8">
+        <f t="shared" si="2"/>
         <v>183265.95</v>
       </c>
-      <c r="F7" s="10">
-        <f t="shared" si="2"/>
-        <v>82469.677500000005</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="F7" s="23">
+        <f t="shared" si="5"/>
+        <v>39.989343355926181</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H7" s="8">
         <v>14190.75</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="8">
         <v>0</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="8">
         <v>3657.15</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="8">
         <f t="shared" si="3"/>
         <v>17847.900000000001</v>
       </c>
-      <c r="K7" s="10">
+      <c r="L7" s="8">
         <v>1037.4000000000001</v>
       </c>
-      <c r="L7" s="10">
+      <c r="M7" s="8">
         <v>71.400000000000006</v>
       </c>
-      <c r="M7" s="10">
+      <c r="N7" s="8">
         <v>0</v>
       </c>
-      <c r="N7" s="10">
+      <c r="O7" s="8">
         <v>1000</v>
       </c>
-      <c r="O7" s="11">
+      <c r="P7" s="9">
         <f t="shared" si="0"/>
         <v>-37.400000000000091</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>45627</v>
-      </c>
-      <c r="B8" s="10">
+        <f t="shared" si="1"/>
+        <v>45630</v>
+      </c>
+      <c r="B8" s="8">
         <v>53708.55</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>8.4</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>18012.75</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="1"/>
+      <c r="E8" s="8">
+        <f t="shared" si="2"/>
         <v>71729.700000000012</v>
       </c>
-      <c r="F8" s="10">
-        <f t="shared" si="2"/>
-        <v>32278.365000000005</v>
-      </c>
-      <c r="G8" s="10">
+      <c r="F8" s="23">
+        <f t="shared" si="5"/>
+        <v>25.111982902479724</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H8" s="8">
         <v>7697.55</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="8">
         <v>1.05</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="8">
         <v>825.3</v>
       </c>
-      <c r="J8" s="10">
+      <c r="K8" s="8">
         <f t="shared" si="3"/>
         <v>8523.9</v>
       </c>
-      <c r="K8" s="10">
+      <c r="L8" s="8">
         <v>1050</v>
       </c>
-      <c r="L8" s="10">
+      <c r="M8" s="8">
         <v>0</v>
       </c>
-      <c r="M8" s="10">
+      <c r="N8" s="8">
         <v>0</v>
       </c>
-      <c r="N8" s="10">
+      <c r="O8" s="8">
         <v>1000</v>
       </c>
-      <c r="O8" s="11">
+      <c r="P8" s="9">
         <f t="shared" si="0"/>
         <v>-50</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>45658</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10" t="str">
-        <f>IF(O9&gt;0,"",IF(SQRT(O9^2)&gt;N9*0.05,SQRT(O9^2),""))</f>
-        <v/>
-      </c>
-      <c r="N9" s="10">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="20" t="str">
+        <f t="shared" ref="F3:F13" si="7">IFERROR(D9/E9,"")</f>
+        <v/>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8" t="str">
+        <f>IF(P9&gt;0,"",IF(SQRT(P9^2)&gt;O9*0.05,SQRT(P9^2),""))</f>
+        <v/>
+      </c>
+      <c r="O9" s="8">
         <v>1000</v>
       </c>
-      <c r="O9" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>45689</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10" t="str">
+      <c r="P9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="20" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="N10" s="10">
+      <c r="O10" s="8">
         <v>1000</v>
       </c>
-      <c r="O10" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>45717</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="12" t="str">
+      <c r="P10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="N11" s="14">
+      <c r="O11" s="12">
         <v>1000</v>
       </c>
-      <c r="O11" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>45748</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="13" t="str">
+      <c r="P11" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="21" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="11" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="N12" s="15">
+      <c r="O12" s="13">
         <v>300</v>
       </c>
-      <c r="O12" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>45778</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="10" t="str">
+      <c r="P12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="N13" s="12">
+      <c r="O13" s="10">
         <v>300</v>
       </c>
-      <c r="O13" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+      <c r="P13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="H15" s="19"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O13" xr:uid="{74ACD048-E26D-43F8-8A45-756E0CC9B87A}"/>
+  <autoFilter ref="A1:P13" xr:uid="{74ACD048-E26D-43F8-8A45-756E0CC9B87A}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1395,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D3E410-0106-4F7F-854D-002E584BAB18}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1518,7 @@
         <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>15</v>
@@ -1463,443 +1531,454 @@
       <c r="A2" s="5">
         <v>45444</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>5845.19</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>2757.87</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <v>213.77</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="8">
         <f>B2+C2+D2</f>
         <v>8816.83</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <v>4795.76</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="8">
         <v>1252.19</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="8">
         <v>687.8</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="8">
         <f>687.8+4795.76+1252.19</f>
         <v>6735.75</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="8">
         <v>11499.84</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="8">
         <v>1839.97</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="8">
         <v>0</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="8">
         <f>N2-E2-I2-J2-K2-L2</f>
         <v>715.2300000000007</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="9">
         <v>29607.62</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>45474</v>
-      </c>
-      <c r="B3" s="10">
+        <f t="shared" ref="A3:A13" si="0">IF(B3="","",A2+31)</f>
+        <v>45475</v>
+      </c>
+      <c r="B3" s="8">
         <v>10963.55</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>3280.98</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>566.88</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" ref="E3:E8" si="0">B3+C3+D3</f>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E8" si="1">B3+C3+D3</f>
         <v>14811.409999999998</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>5014.92</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>803.69</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="8">
         <v>1418.97</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <f>803.69+5014.92+1418.97</f>
         <v>7237.5800000000008</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <v>11618.83</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <v>38.21</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="8">
         <v>1397.76</v>
       </c>
-      <c r="M3" s="10">
-        <f t="shared" ref="M3:M8" si="1">N3-E3-I3-J3-K3-L3</f>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M8" si="2">N3-E3-I3-J3-K3-L3</f>
         <v>2682.0499999999984</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="9">
         <f>37785.84</f>
         <v>37785.839999999997</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>45505</v>
-      </c>
-      <c r="B4" s="12">
+        <f t="shared" si="0"/>
+        <v>45506</v>
+      </c>
+      <c r="B4" s="10">
         <v>49458.33</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>2936.55</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>3243.77</v>
       </c>
-      <c r="E4" s="12">
-        <f t="shared" si="0"/>
+      <c r="E4" s="10">
+        <f t="shared" si="1"/>
         <v>55638.65</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>5886.19</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <v>394.46</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <v>1560.16</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="10">
         <f>394.46+5886.19+1560.16</f>
         <v>7840.8099999999995</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <v>12187.84</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="10">
         <v>2369.86</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <v>2880.36</v>
       </c>
-      <c r="M4" s="12">
-        <f t="shared" si="1"/>
+      <c r="M4" s="10">
+        <f t="shared" si="2"/>
         <v>7579.0800000000054</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="15">
         <v>88496.6</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>45536</v>
-      </c>
-      <c r="B5" s="13">
+        <f t="shared" si="0"/>
+        <v>45537</v>
+      </c>
+      <c r="B5" s="11">
         <v>80220.710000000006</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>4505.76</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <v>5056.96</v>
       </c>
-      <c r="E5" s="13">
-        <f t="shared" si="0"/>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
         <v>89783.430000000008</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <v>8186.26</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <v>761.33</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>1844.96</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="11">
         <f>761.33+8186.26+1844.96</f>
         <v>10792.55</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="11">
         <v>38286.31</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="11">
         <v>3152.54</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="11">
         <v>4225.09</v>
       </c>
-      <c r="M5" s="13">
-        <f t="shared" si="1"/>
+      <c r="M5" s="11">
+        <f t="shared" si="2"/>
         <v>20925.34</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="14">
         <v>167165.26</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>45566</v>
-      </c>
-      <c r="B6" s="10">
+        <f t="shared" si="0"/>
+        <v>45568</v>
+      </c>
+      <c r="B6" s="8">
         <v>64048.800000000003</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>261.38</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>4697.2299999999996</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="0"/>
+      <c r="E6" s="8">
+        <f t="shared" si="1"/>
         <v>69007.41</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>5608.73</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>32.56</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="8">
         <v>1472.46</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <f>32.56+5608.73+1472.46</f>
         <v>7113.75</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <v>40326.29</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="8">
         <v>2568.3000000000002</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="8">
         <v>7637.38</v>
       </c>
-      <c r="M6" s="10">
-        <f t="shared" si="1"/>
+      <c r="M6" s="8">
+        <f t="shared" si="2"/>
         <v>27970.19</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="9">
         <v>154623.32</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>45597</v>
-      </c>
-      <c r="B7" s="10">
+        <f t="shared" si="0"/>
+        <v>45599</v>
+      </c>
+      <c r="B7" s="8">
         <v>61153.27</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>0</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>4075.06</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="0"/>
+      <c r="E7" s="8">
+        <f t="shared" si="1"/>
         <v>65228.329999999994</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>5765.35</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="8">
         <v>1485.8</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <f>5765.35+1485.8</f>
         <v>7251.1500000000005</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <v>37700.57</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="8">
         <v>2594.7600000000002</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <v>0</v>
       </c>
-      <c r="M7" s="10">
-        <f t="shared" si="1"/>
+      <c r="M7" s="8">
+        <f t="shared" si="2"/>
         <v>15910.110000000002</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="9">
         <v>128684.92</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>45627</v>
-      </c>
-      <c r="B8" s="10">
+        <f t="shared" si="0"/>
+        <v>45630</v>
+      </c>
+      <c r="B8" s="8">
         <v>29192.21</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>26.07</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>979.02</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="0"/>
+      <c r="E8" s="8">
+        <f t="shared" si="1"/>
         <v>30197.3</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>3056.94</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <v>0.41</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="8">
         <v>327.75</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <f>0.41+3056.94+327.75</f>
         <v>3385.1</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="8">
         <v>37299.699999999997</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="8">
         <v>0</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="8">
         <v>0</v>
       </c>
-      <c r="M8" s="10">
-        <f t="shared" si="1"/>
+      <c r="M8" s="8">
+        <f t="shared" si="2"/>
         <v>2773.489999999998</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="9">
         <v>73655.59</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>45658</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10">
+      <c r="A9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8">
         <v>1000</v>
       </c>
-      <c r="N9" s="11" t="str">
+      <c r="N9" s="9" t="str">
         <f>IF(J9="","",M9-J9)</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>45689</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10">
+      <c r="A10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8">
         <v>1000</v>
       </c>
-      <c r="N10" s="11" t="str">
+      <c r="N10" s="9" t="str">
         <f>IF(J10="","",M10-J10)</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>45717</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14">
+      <c r="A11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12">
         <v>1000</v>
       </c>
-      <c r="N11" s="17" t="str">
+      <c r="N11" s="15" t="str">
         <f>IF(J11="","",M11-J11)</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>45748</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15">
+      <c r="A12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13">
         <v>300</v>
       </c>
-      <c r="N12" s="16" t="str">
+      <c r="N12" s="14" t="str">
         <f>IF(J12="","",M12-J12)</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>45778</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12">
+      <c r="A13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10">
         <v>300</v>
       </c>
-      <c r="N13" s="11" t="str">
+      <c r="N13" s="9" t="str">
         <f>IF(J13="","",M13-J13)</f>
         <v/>
       </c>

</xml_diff>